<commit_message>
master 进行CRN 8通道 mel谱
</commit_message>
<xml_diff>
--- a/evaluate.xlsx
+++ b/evaluate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21730" windowHeight="10330"/>
+    <workbookView windowWidth="28125" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+  <si>
+    <t>loss</t>
+  </si>
+  <si>
+    <t>ckpt模型</t>
+  </si>
   <si>
     <t>平均帧错误数</t>
   </si>
@@ -94,6 +100,30 @@
   </si>
   <si>
     <t>24.86</t>
+  </si>
+  <si>
+    <t>crn_diff_loss_multi_channel_complex</t>
+  </si>
+  <si>
+    <t>0.6959</t>
+  </si>
+  <si>
+    <t>168.3939</t>
+  </si>
+  <si>
+    <t>16.8225</t>
+  </si>
+  <si>
+    <t>crn_diff_loss_single_channel_mel</t>
+  </si>
+  <si>
+    <t>0.721055</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0.09990</t>
   </si>
 </sst>
 </file>
@@ -101,10 +131,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -116,6 +146,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -129,23 +181,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -156,29 +217,6 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -231,7 +269,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -239,14 +277,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -268,187 +298,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -488,6 +518,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -534,21 +579,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -567,10 +597,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -579,133 +609,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -713,8 +743,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1064,142 +1094,183 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="46.8181818181818" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.8181818181818" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22" style="1" customWidth="1"/>
-    <col min="5" max="5" width="73" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="46.8166666666667" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.8166666666667" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22" style="1" customWidth="1"/>
+    <col min="6" max="6" width="73" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:5">
+    <row r="1" spans="2:6">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="2" ht="24" customHeight="1" spans="1:5">
+    <row r="2" ht="24" customHeight="1" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="3:5">
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="2:4">
-      <c r="B3" s="1" t="s">
+    <row r="4" spans="3:5">
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="4" spans="2:4">
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
+    <row r="5" spans="3:5">
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
-      <c r="B5" s="1" t="s">
+    <row r="6" spans="3:5">
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>6</v>
+      <c r="D8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
-      <c r="B6" s="1" t="s">
+    <row r="9" spans="3:5">
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5">
+      <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5">
+      <c r="C11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
+      <c r="D11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>17</v>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="9" spans="2:4">
-      <c r="B9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4">
-      <c r="B10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4">
-      <c r="B11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>25</v>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1218,7 +1289,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1235,7 +1306,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
multi channel mel -win320 作为输入
</commit_message>
<xml_diff>
--- a/evaluate.xlsx
+++ b/evaluate.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
   <si>
     <t>win len</t>
   </si>
@@ -102,18 +102,33 @@
     <t>32.455</t>
   </si>
   <si>
+    <t>crn_multi_channel_mel</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
     <t>199.18</t>
   </si>
   <si>
     <t>24.86</t>
   </si>
   <si>
-    <t>crn_diff_loss_multi_channel_complex_15epoch</t>
-  </si>
-  <si>
     <t>320</t>
   </si>
   <si>
+    <t>0.713264</t>
+  </si>
+  <si>
+    <t>264.39092</t>
+  </si>
+  <si>
+    <t>26.4126803</t>
+  </si>
+  <si>
+    <t>crn_multi_channel_complex_15epoch</t>
+  </si>
+  <si>
     <t>0.6959</t>
   </si>
   <si>
@@ -123,7 +138,7 @@
     <t>16.8225</t>
   </si>
   <si>
-    <t>crn_diff_loss_multi_channel_complex_50epoch</t>
+    <t>crn_multi_channel_complex_50epoch</t>
   </si>
   <si>
     <t>0.6863</t>
@@ -144,7 +159,7 @@
     <t>33.2096</t>
   </si>
   <si>
-    <t>crn_diff_loss_single_channel_mel</t>
+    <t>crn_single_channel_mel</t>
   </si>
   <si>
     <t>0.721055</t>
@@ -161,9 +176,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -189,6 +204,83 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -198,22 +290,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -221,99 +314,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -328,12 +343,180 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -341,174 +524,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -519,26 +534,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -557,17 +552,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -591,7 +582,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -599,8 +590,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -619,6 +625,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -627,10 +642,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -639,10 +654,10 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -651,121 +666,121 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1124,20 +1139,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="52.875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="35.75" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7583333333333" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.8166666666667" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16" style="1" customWidth="1"/>
     <col min="7" max="7" width="73" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
@@ -1265,89 +1280,121 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="4:6">
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="D11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>34</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>41</v>
+      <c r="B16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="1" t="s">
+    <row r="18" spans="1:6">
+      <c r="A18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>45</v>
+      <c r="E18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
multi channel mel -win320 作为输入 网络最后的激活函数由softmax换为sigmoid
改frame_level_label，用卷积方式实现
</commit_message>
<xml_diff>
--- a/evaluate.xlsx
+++ b/evaluate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540"/>
+    <workbookView windowWidth="21730" windowHeight="10330"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
   <si>
     <t>win len</t>
   </si>
@@ -169,6 +169,18 @@
   </si>
   <si>
     <t>29.15339</t>
+  </si>
+  <si>
+    <t>crn_multi_channel_complex_sigmoid_50epoch</t>
+  </si>
+  <si>
+    <t>0.81676</t>
+  </si>
+  <si>
+    <t>141.93927</t>
+  </si>
+  <si>
+    <t>14.1797</t>
   </si>
 </sst>
 </file>
@@ -190,6 +202,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -197,13 +231,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
@@ -211,42 +254,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -265,14 +301,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -298,13 +326,12 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -312,23 +339,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -343,187 +355,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -534,6 +546,32 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -552,13 +590,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -596,36 +638,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -642,10 +654,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -654,133 +666,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1139,19 +1151,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="35.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="45.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.87272727272727" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.8727272727273" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6272727272727" style="1" customWidth="1"/>
     <col min="6" max="6" width="16" style="1" customWidth="1"/>
     <col min="7" max="7" width="73" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="1"/>
@@ -1395,6 +1407,26 @@
       </c>
       <c r="F18" s="1" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1413,7 +1445,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1430,7 +1462,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>